<commit_message>
Actualización de formato antiguo.
</commit_message>
<xml_diff>
--- a/public/formato_bac_viejo.xlsx
+++ b/public/formato_bac_viejo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\uc\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5892CB5B-FF63-47FE-9EF1-E15AAF2DAD2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D889421-9C74-44F2-944D-4D44E0A1A00F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="10" r:id="rId1"/>
@@ -616,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -831,14 +831,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -854,18 +846,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -874,19 +854,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -924,24 +892,71 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -963,60 +978,16 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1037,22 +1008,21 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1063,15 +1033,53 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1749,50 +1757,50 @@
   <dimension ref="A1:L74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:L6"/>
+      <selection activeCell="H11" sqref="H11:K70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="23.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="3.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="23.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
       <c r="L1" s="58"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
       <c r="G2" s="58"/>
       <c r="H2" s="58"/>
       <c r="I2" s="22"/>
@@ -1800,23 +1808,23 @@
       <c r="K2" s="22"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="101" t="s">
+    <row r="3" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
       <c r="L3" s="59"/>
     </row>
-    <row r="4" spans="1:12" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -1829,63 +1837,63 @@
       <c r="J4" s="24"/>
       <c r="K4" s="23"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
       <c r="J5" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="97"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L5" s="90"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
       <c r="I6" s="48"/>
       <c r="J6" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K6" s="106"/>
+      <c r="L6" s="106"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
       <c r="I7" s="47"/>
       <c r="J7" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-    </row>
-    <row r="8" spans="1:12" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K7" s="90"/>
+      <c r="L7" s="90"/>
+    </row>
+    <row r="8" spans="1:12" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -1898,45 +1906,45 @@
       <c r="J8" s="26"/>
       <c r="K8" s="23"/>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="107" t="s">
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="113" t="s">
+      <c r="D9" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="115" t="s">
+      <c r="E9" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="117" t="s">
+      <c r="F9" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="117" t="s">
+      <c r="G9" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="119" t="s">
+      <c r="H9" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="120"/>
-      <c r="J9" s="119" t="s">
+      <c r="I9" s="104"/>
+      <c r="J9" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="120"/>
-    </row>
-    <row r="10" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="108"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="118"/>
+      <c r="K9" s="104"/>
+    </row>
+    <row r="10" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="92"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="49" t="s">
         <v>7</v>
       </c>
@@ -1950,1282 +1958,1282 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="64">
         <v>1</v>
       </c>
       <c r="B11" s="65"/>
       <c r="C11" s="66"/>
       <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="69"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="134"/>
       <c r="H11" s="67"/>
-      <c r="I11" s="60" t="str">
+      <c r="I11" s="136" t="str">
         <f>IF(H11="","",IF(H11=0,"cero",IF(H11=5,"cinco",IF(H11=6,"seis",IF(H11=7,"siete",IF(H11=8,"ocho",IF(H11=9,"nueve",IF(H11=10,"diez",IF(H11="NC","NC")))))))))</f>
         <v/>
       </c>
       <c r="J11" s="67"/>
-      <c r="K11" s="60" t="str">
+      <c r="K11" s="136" t="str">
         <f>IF(J11="","",IF(J11=0,"cero",IF(J11=5,"cinco",IF(J11=6,"seis",IF(J11=7,"siete",IF(J11=8,"ocho",IF(J11=9,"nueve",IF(J11=10,"diez",IF(J11="NC","NC")))))))))</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="70">
+    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="68">
         <v>2</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="60" t="str">
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="129"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="136" t="str">
         <f t="shared" ref="I12:I70" si="0">IF(H12="","",IF(H12=0,"cero",IF(H12=5,"cinco",IF(H12=6,"seis",IF(H12=7,"siete",IF(H12=8,"ocho",IF(H12=9,"nueve",IF(H12=10,"diez",IF(H12="NC","NC")))))))))</f>
         <v/>
       </c>
-      <c r="J12" s="73"/>
-      <c r="K12" s="60" t="str">
+      <c r="J12" s="71"/>
+      <c r="K12" s="136" t="str">
         <f t="shared" ref="K12:K70" si="1">IF(J12="","",IF(J12=0,"cero",IF(J12=5,"cinco",IF(J12=6,"seis",IF(J12=7,"siete",IF(J12=8,"ocho",IF(J12=9,"nueve",IF(J12=10,"diez",IF(J12="NC","NC")))))))))</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="70">
+    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="68">
         <v>3</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J13" s="73"/>
-      <c r="K13" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="70">
+      <c r="B13" s="69"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J13" s="71"/>
+      <c r="K13" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="68">
         <v>4</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J14" s="73"/>
-      <c r="K14" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="70">
+      <c r="B14" s="69"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="129"/>
+      <c r="G14" s="135"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J14" s="71"/>
+      <c r="K14" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="68">
         <v>5</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J15" s="73"/>
-      <c r="K15" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="70">
+      <c r="B15" s="69"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J15" s="71"/>
+      <c r="K15" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="68">
         <v>6</v>
       </c>
-      <c r="B16" s="71"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J16" s="73"/>
-      <c r="K16" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="70">
+      <c r="B16" s="69"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="129"/>
+      <c r="G16" s="130"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J16" s="71"/>
+      <c r="K16" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="68">
         <v>7</v>
       </c>
-      <c r="B17" s="71"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J17" s="73"/>
-      <c r="K17" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="70">
+      <c r="B17" s="69"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="129"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J17" s="71"/>
+      <c r="K17" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="68">
         <v>8</v>
       </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J18" s="73"/>
-      <c r="K18" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="70">
+      <c r="B18" s="69"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="129"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J18" s="71"/>
+      <c r="K18" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="68">
         <v>9</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J19" s="73"/>
-      <c r="K19" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="70">
+      <c r="B19" s="69"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="129"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J19" s="71"/>
+      <c r="K19" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="68">
         <v>10</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="70">
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="126"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J20" s="71"/>
+      <c r="K20" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="68">
         <v>11</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J21" s="73"/>
-      <c r="K21" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="70">
+      <c r="B21" s="69"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="126"/>
+      <c r="F21" s="129"/>
+      <c r="G21" s="135"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J21" s="71"/>
+      <c r="K21" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="68">
         <v>12</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J22" s="73"/>
-      <c r="K22" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70">
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="126"/>
+      <c r="F22" s="129"/>
+      <c r="G22" s="135"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J22" s="71"/>
+      <c r="K22" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="68">
         <v>13</v>
       </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J23" s="73"/>
-      <c r="K23" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="70">
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="135"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J23" s="71"/>
+      <c r="K23" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="68">
         <v>14</v>
       </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J24" s="73"/>
-      <c r="K24" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="70">
+      <c r="B24" s="72"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="126"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J24" s="71"/>
+      <c r="K24" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="68">
         <v>15</v>
       </c>
-      <c r="B25" s="77"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J25" s="73"/>
-      <c r="K25" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="70">
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="129"/>
+      <c r="G25" s="135"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J25" s="71"/>
+      <c r="K25" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="68">
         <v>16</v>
       </c>
-      <c r="B26" s="77"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="82"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="81"/>
-      <c r="I26" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J26" s="73"/>
-      <c r="K26" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="70">
+      <c r="B26" s="72"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="126"/>
+      <c r="F26" s="131"/>
+      <c r="G26" s="130"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J26" s="71"/>
+      <c r="K26" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="68">
         <v>17</v>
       </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J27" s="73"/>
-      <c r="K27" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="70">
+      <c r="B27" s="72"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="126"/>
+      <c r="F27" s="129"/>
+      <c r="G27" s="135"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J27" s="71"/>
+      <c r="K27" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="68">
         <v>18</v>
       </c>
-      <c r="B28" s="77"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J28" s="73"/>
-      <c r="K28" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="70">
+      <c r="B28" s="72"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="126"/>
+      <c r="F28" s="131"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J28" s="71"/>
+      <c r="K28" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="68">
         <v>19</v>
       </c>
-      <c r="B29" s="77"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="82"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J29" s="73"/>
-      <c r="K29" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="70">
+      <c r="B29" s="72"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="131"/>
+      <c r="G29" s="130"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J29" s="71"/>
+      <c r="K29" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="68">
         <v>20</v>
       </c>
-      <c r="B30" s="77"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J30" s="73"/>
-      <c r="K30" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="70">
+      <c r="B30" s="72"/>
+      <c r="C30" s="73"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="126"/>
+      <c r="F30" s="131"/>
+      <c r="G30" s="130"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J30" s="71"/>
+      <c r="K30" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="68">
         <v>21</v>
       </c>
-      <c r="B31" s="77"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="81"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="81"/>
-      <c r="I31" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J31" s="83"/>
-      <c r="K31" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="70">
+      <c r="B31" s="72"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="126"/>
+      <c r="F31" s="131"/>
+      <c r="G31" s="130"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J31" s="75"/>
+      <c r="K31" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="68">
         <v>22</v>
       </c>
-      <c r="B32" s="77"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="80"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="79"/>
-      <c r="I32" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J32" s="73"/>
-      <c r="K32" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70">
+      <c r="B32" s="72"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="126"/>
+      <c r="F32" s="129"/>
+      <c r="G32" s="135"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J32" s="71"/>
+      <c r="K32" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="68">
         <v>23</v>
       </c>
-      <c r="B33" s="77"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="80"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J33" s="73"/>
-      <c r="K33" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="70">
+      <c r="B33" s="72"/>
+      <c r="C33" s="73"/>
+      <c r="D33" s="73"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="129"/>
+      <c r="G33" s="135"/>
+      <c r="H33" s="75"/>
+      <c r="I33" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J33" s="71"/>
+      <c r="K33" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="68">
         <v>24</v>
       </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="82"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J34" s="84"/>
-      <c r="K34" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="70">
+      <c r="B34" s="72"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="126"/>
+      <c r="F34" s="131"/>
+      <c r="G34" s="130"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J34" s="76"/>
+      <c r="K34" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="68">
         <v>25</v>
       </c>
-      <c r="B35" s="77"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J35" s="73"/>
-      <c r="K35" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="70">
+      <c r="B35" s="72"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="129"/>
+      <c r="G35" s="135"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J35" s="71"/>
+      <c r="K35" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="68">
         <v>26</v>
       </c>
-      <c r="B36" s="77"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J36" s="84"/>
-      <c r="K36" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="70">
+      <c r="B36" s="72"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="126"/>
+      <c r="F36" s="131"/>
+      <c r="G36" s="130"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J36" s="76"/>
+      <c r="K36" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="68">
         <v>27</v>
       </c>
-      <c r="B37" s="77"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J37" s="84"/>
-      <c r="K37" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="70">
+      <c r="B37" s="72"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="126"/>
+      <c r="F37" s="131"/>
+      <c r="G37" s="130"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J37" s="76"/>
+      <c r="K37" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="68">
         <v>28</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="81"/>
-      <c r="I38" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J38" s="84"/>
-      <c r="K38" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="70">
+      <c r="B38" s="72"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="126"/>
+      <c r="F38" s="131"/>
+      <c r="G38" s="130"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J38" s="76"/>
+      <c r="K38" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="68">
         <v>29</v>
       </c>
-      <c r="B39" s="77"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J39" s="73"/>
-      <c r="K39" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="70">
+      <c r="B39" s="72"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="126"/>
+      <c r="F39" s="129"/>
+      <c r="G39" s="135"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J39" s="71"/>
+      <c r="K39" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="68">
         <v>30</v>
       </c>
-      <c r="B40" s="77"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="79"/>
-      <c r="I40" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J40" s="73"/>
-      <c r="K40" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="70">
+      <c r="B40" s="72"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="126"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="135"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J40" s="71"/>
+      <c r="K40" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="68">
         <v>31</v>
       </c>
-      <c r="B41" s="77"/>
-      <c r="C41" s="78"/>
-      <c r="D41" s="78"/>
-      <c r="E41" s="79"/>
-      <c r="F41" s="80"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J41" s="73"/>
-      <c r="K41" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="70">
+      <c r="B41" s="72"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="126"/>
+      <c r="F41" s="129"/>
+      <c r="G41" s="135"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J41" s="71"/>
+      <c r="K41" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="68">
         <v>32</v>
       </c>
-      <c r="B42" s="77"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="82"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J42" s="84"/>
-      <c r="K42" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="70">
+      <c r="B42" s="72"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="126"/>
+      <c r="F42" s="131"/>
+      <c r="G42" s="130"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J42" s="76"/>
+      <c r="K42" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="68">
         <v>33</v>
       </c>
-      <c r="B43" s="77"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="80"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J43" s="73"/>
-      <c r="K43" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="70">
+      <c r="B43" s="72"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="126"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="135"/>
+      <c r="H43" s="75"/>
+      <c r="I43" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J43" s="71"/>
+      <c r="K43" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="68">
         <v>34</v>
       </c>
-      <c r="B44" s="77"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="76"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J44" s="84"/>
-      <c r="K44" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="70">
+      <c r="B44" s="72"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="126"/>
+      <c r="F44" s="131"/>
+      <c r="G44" s="130"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J44" s="76"/>
+      <c r="K44" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="68">
         <v>35</v>
       </c>
-      <c r="B45" s="77"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="78"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="80"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="79"/>
-      <c r="I45" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J45" s="73"/>
-      <c r="K45" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="70">
+      <c r="B45" s="72"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="126"/>
+      <c r="F45" s="129"/>
+      <c r="G45" s="135"/>
+      <c r="H45" s="75"/>
+      <c r="I45" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J45" s="71"/>
+      <c r="K45" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="68">
         <v>36</v>
       </c>
-      <c r="B46" s="85"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="81"/>
-      <c r="I46" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J46" s="73"/>
-      <c r="K46" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="70">
+      <c r="B46" s="77"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="126"/>
+      <c r="F46" s="131"/>
+      <c r="G46" s="130"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J46" s="71"/>
+      <c r="K46" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="68">
         <v>37</v>
       </c>
-      <c r="B47" s="85"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="78"/>
-      <c r="E47" s="81"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="76"/>
-      <c r="H47" s="81"/>
-      <c r="I47" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J47" s="73"/>
-      <c r="K47" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="70">
+      <c r="B47" s="77"/>
+      <c r="C47" s="73"/>
+      <c r="D47" s="73"/>
+      <c r="E47" s="126"/>
+      <c r="F47" s="131"/>
+      <c r="G47" s="130"/>
+      <c r="H47" s="74"/>
+      <c r="I47" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J47" s="71"/>
+      <c r="K47" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="68">
         <v>38</v>
       </c>
-      <c r="B48" s="85"/>
-      <c r="C48" s="78"/>
-      <c r="D48" s="78"/>
-      <c r="E48" s="81"/>
-      <c r="F48" s="82"/>
-      <c r="G48" s="76"/>
-      <c r="H48" s="81"/>
-      <c r="I48" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J48" s="73"/>
-      <c r="K48" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="70">
+      <c r="B48" s="77"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="126"/>
+      <c r="F48" s="131"/>
+      <c r="G48" s="130"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J48" s="71"/>
+      <c r="K48" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="68">
         <v>39</v>
       </c>
-      <c r="B49" s="85"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="78"/>
-      <c r="E49" s="81"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="76"/>
-      <c r="H49" s="81"/>
-      <c r="I49" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J49" s="73"/>
-      <c r="K49" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="70">
+      <c r="B49" s="77"/>
+      <c r="C49" s="73"/>
+      <c r="D49" s="73"/>
+      <c r="E49" s="126"/>
+      <c r="F49" s="131"/>
+      <c r="G49" s="130"/>
+      <c r="H49" s="74"/>
+      <c r="I49" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J49" s="71"/>
+      <c r="K49" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="68">
         <f>A49+1</f>
         <v>40</v>
       </c>
-      <c r="B50" s="85"/>
-      <c r="C50" s="78"/>
-      <c r="D50" s="78"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J50" s="73"/>
-      <c r="K50" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="70">
+      <c r="B50" s="77"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="126"/>
+      <c r="F50" s="131"/>
+      <c r="G50" s="130"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J50" s="71"/>
+      <c r="K50" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="68">
         <f t="shared" ref="A51:A59" si="2">A50+1</f>
         <v>41</v>
       </c>
-      <c r="B51" s="85"/>
-      <c r="C51" s="78"/>
-      <c r="D51" s="78"/>
-      <c r="E51" s="81"/>
-      <c r="F51" s="82"/>
-      <c r="G51" s="76"/>
-      <c r="H51" s="81"/>
-      <c r="I51" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J51" s="73"/>
-      <c r="K51" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="70">
+      <c r="B51" s="77"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
+      <c r="E51" s="126"/>
+      <c r="F51" s="131"/>
+      <c r="G51" s="130"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J51" s="71"/>
+      <c r="K51" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="68">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="B52" s="85"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="78"/>
-      <c r="E52" s="81"/>
-      <c r="F52" s="82"/>
-      <c r="G52" s="76"/>
-      <c r="H52" s="81"/>
-      <c r="I52" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J52" s="73"/>
-      <c r="K52" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="70">
+      <c r="B52" s="77"/>
+      <c r="C52" s="73"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="126"/>
+      <c r="F52" s="131"/>
+      <c r="G52" s="130"/>
+      <c r="H52" s="74"/>
+      <c r="I52" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J52" s="71"/>
+      <c r="K52" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="68">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="B53" s="85"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="78"/>
-      <c r="E53" s="81"/>
-      <c r="F53" s="82"/>
-      <c r="G53" s="76"/>
-      <c r="H53" s="81"/>
-      <c r="I53" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J53" s="73"/>
-      <c r="K53" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="70">
+      <c r="B53" s="77"/>
+      <c r="C53" s="73"/>
+      <c r="D53" s="73"/>
+      <c r="E53" s="126"/>
+      <c r="F53" s="131"/>
+      <c r="G53" s="130"/>
+      <c r="H53" s="74"/>
+      <c r="I53" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J53" s="71"/>
+      <c r="K53" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="68">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="B54" s="85"/>
-      <c r="C54" s="78"/>
-      <c r="D54" s="78"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="82"/>
-      <c r="G54" s="76"/>
-      <c r="H54" s="81"/>
-      <c r="I54" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J54" s="73"/>
-      <c r="K54" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="70">
+      <c r="B54" s="77"/>
+      <c r="C54" s="73"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="126"/>
+      <c r="F54" s="131"/>
+      <c r="G54" s="130"/>
+      <c r="H54" s="74"/>
+      <c r="I54" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J54" s="71"/>
+      <c r="K54" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="68">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="B55" s="85"/>
-      <c r="C55" s="78"/>
-      <c r="D55" s="78"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="82"/>
-      <c r="G55" s="76"/>
-      <c r="H55" s="81"/>
-      <c r="I55" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J55" s="73"/>
-      <c r="K55" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="70">
+      <c r="B55" s="77"/>
+      <c r="C55" s="73"/>
+      <c r="D55" s="73"/>
+      <c r="E55" s="126"/>
+      <c r="F55" s="131"/>
+      <c r="G55" s="130"/>
+      <c r="H55" s="74"/>
+      <c r="I55" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J55" s="71"/>
+      <c r="K55" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="68">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="B56" s="85"/>
-      <c r="C56" s="78"/>
-      <c r="D56" s="78"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="82"/>
-      <c r="G56" s="76"/>
-      <c r="H56" s="81"/>
-      <c r="I56" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J56" s="73"/>
-      <c r="K56" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="70">
+      <c r="B56" s="77"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="126"/>
+      <c r="F56" s="131"/>
+      <c r="G56" s="130"/>
+      <c r="H56" s="74"/>
+      <c r="I56" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J56" s="71"/>
+      <c r="K56" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="68">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="B57" s="85"/>
-      <c r="C57" s="78"/>
-      <c r="D57" s="78"/>
-      <c r="E57" s="81"/>
-      <c r="F57" s="82"/>
-      <c r="G57" s="76"/>
-      <c r="H57" s="81"/>
-      <c r="I57" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J57" s="73"/>
-      <c r="K57" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="70">
+      <c r="B57" s="77"/>
+      <c r="C57" s="73"/>
+      <c r="D57" s="73"/>
+      <c r="E57" s="126"/>
+      <c r="F57" s="131"/>
+      <c r="G57" s="130"/>
+      <c r="H57" s="74"/>
+      <c r="I57" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J57" s="71"/>
+      <c r="K57" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="68">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="B58" s="85"/>
-      <c r="C58" s="78"/>
-      <c r="D58" s="78"/>
-      <c r="E58" s="81"/>
-      <c r="F58" s="82"/>
-      <c r="G58" s="76"/>
-      <c r="H58" s="81"/>
-      <c r="I58" s="60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J58" s="73"/>
-      <c r="K58" s="60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="70">
+      <c r="B58" s="77"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="126"/>
+      <c r="F58" s="131"/>
+      <c r="G58" s="130"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="136" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J58" s="71"/>
+      <c r="K58" s="136" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="68">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="B59" s="85"/>
-      <c r="C59" s="78"/>
-      <c r="D59" s="78"/>
-      <c r="E59" s="81"/>
-      <c r="F59" s="82"/>
-      <c r="G59" s="76"/>
-      <c r="H59" s="81"/>
-      <c r="I59" s="60" t="str">
+      <c r="B59" s="77"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="126"/>
+      <c r="F59" s="131"/>
+      <c r="G59" s="130"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="136" t="str">
         <f t="shared" ref="I59:I69" si="3">IF(H59="","",IF(H59=0,"cero",IF(H59=5,"cinco",IF(H59=6,"seis",IF(H59=7,"siete",IF(H59=8,"ocho",IF(H59=9,"nueve",IF(H59=10,"diez",IF(H59="NC","NC")))))))))</f>
         <v/>
       </c>
-      <c r="J59" s="73"/>
-      <c r="K59" s="60" t="str">
+      <c r="J59" s="71"/>
+      <c r="K59" s="136" t="str">
         <f t="shared" ref="K59:K69" si="4">IF(J59="","",IF(J59=0,"cero",IF(J59=5,"cinco",IF(J59=6,"seis",IF(J59=7,"siete",IF(J59=8,"ocho",IF(J59=9,"nueve",IF(J59=10,"diez",IF(J59="NC","NC")))))))))</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="86">
+    <row r="60" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="78">
         <v>50</v>
       </c>
-      <c r="B60" s="85"/>
-      <c r="C60" s="78"/>
-      <c r="D60" s="78"/>
-      <c r="E60" s="81"/>
-      <c r="F60" s="82"/>
-      <c r="G60" s="76"/>
-      <c r="H60" s="81"/>
-      <c r="I60" s="60" t="str">
+      <c r="B60" s="77"/>
+      <c r="C60" s="73"/>
+      <c r="D60" s="73"/>
+      <c r="E60" s="126"/>
+      <c r="F60" s="131"/>
+      <c r="G60" s="130"/>
+      <c r="H60" s="74"/>
+      <c r="I60" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J60" s="73"/>
-      <c r="K60" s="60" t="str">
+      <c r="J60" s="71"/>
+      <c r="K60" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="86">
+    <row r="61" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="78">
         <v>51</v>
       </c>
-      <c r="B61" s="85"/>
-      <c r="C61" s="78"/>
-      <c r="D61" s="78"/>
-      <c r="E61" s="81"/>
-      <c r="F61" s="82"/>
-      <c r="G61" s="76"/>
-      <c r="H61" s="81"/>
-      <c r="I61" s="60" t="str">
+      <c r="B61" s="77"/>
+      <c r="C61" s="73"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="126"/>
+      <c r="F61" s="131"/>
+      <c r="G61" s="130"/>
+      <c r="H61" s="74"/>
+      <c r="I61" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J61" s="73"/>
-      <c r="K61" s="60" t="str">
+      <c r="J61" s="71"/>
+      <c r="K61" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="86">
+    <row r="62" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="78">
         <v>52</v>
       </c>
-      <c r="B62" s="85"/>
-      <c r="C62" s="78"/>
-      <c r="D62" s="78"/>
-      <c r="E62" s="81"/>
-      <c r="F62" s="82"/>
-      <c r="G62" s="76"/>
-      <c r="H62" s="81"/>
-      <c r="I62" s="60" t="str">
+      <c r="B62" s="77"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="126"/>
+      <c r="F62" s="131"/>
+      <c r="G62" s="130"/>
+      <c r="H62" s="74"/>
+      <c r="I62" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J62" s="73"/>
-      <c r="K62" s="60" t="str">
+      <c r="J62" s="71"/>
+      <c r="K62" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="86">
+    <row r="63" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="78">
         <v>53</v>
       </c>
-      <c r="B63" s="85"/>
-      <c r="C63" s="78"/>
-      <c r="D63" s="78"/>
-      <c r="E63" s="81"/>
-      <c r="F63" s="82"/>
-      <c r="G63" s="76"/>
-      <c r="H63" s="81"/>
-      <c r="I63" s="60" t="str">
+      <c r="B63" s="77"/>
+      <c r="C63" s="73"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="126"/>
+      <c r="F63" s="131"/>
+      <c r="G63" s="130"/>
+      <c r="H63" s="74"/>
+      <c r="I63" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J63" s="73"/>
-      <c r="K63" s="60" t="str">
+      <c r="J63" s="71"/>
+      <c r="K63" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="86">
+    <row r="64" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="78">
         <v>54</v>
       </c>
-      <c r="B64" s="85"/>
-      <c r="C64" s="78"/>
-      <c r="D64" s="78"/>
-      <c r="E64" s="81"/>
-      <c r="F64" s="82"/>
-      <c r="G64" s="76"/>
-      <c r="H64" s="81"/>
-      <c r="I64" s="60" t="str">
+      <c r="B64" s="77"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="126"/>
+      <c r="F64" s="131"/>
+      <c r="G64" s="130"/>
+      <c r="H64" s="74"/>
+      <c r="I64" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J64" s="73"/>
-      <c r="K64" s="60" t="str">
+      <c r="J64" s="71"/>
+      <c r="K64" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="86">
+    <row r="65" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="78">
         <v>55</v>
       </c>
-      <c r="B65" s="85"/>
-      <c r="C65" s="78"/>
-      <c r="D65" s="78"/>
-      <c r="E65" s="81"/>
-      <c r="F65" s="82"/>
-      <c r="G65" s="76"/>
-      <c r="H65" s="81"/>
-      <c r="I65" s="60" t="str">
+      <c r="B65" s="77"/>
+      <c r="C65" s="73"/>
+      <c r="D65" s="73"/>
+      <c r="E65" s="126"/>
+      <c r="F65" s="131"/>
+      <c r="G65" s="130"/>
+      <c r="H65" s="74"/>
+      <c r="I65" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J65" s="73"/>
-      <c r="K65" s="60" t="str">
+      <c r="J65" s="71"/>
+      <c r="K65" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="86">
+    <row r="66" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="78">
         <v>56</v>
       </c>
-      <c r="B66" s="85"/>
-      <c r="C66" s="78"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="81"/>
-      <c r="F66" s="82"/>
-      <c r="G66" s="76"/>
-      <c r="H66" s="81"/>
-      <c r="I66" s="60" t="str">
+      <c r="B66" s="77"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="126"/>
+      <c r="F66" s="131"/>
+      <c r="G66" s="130"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J66" s="73"/>
-      <c r="K66" s="60" t="str">
+      <c r="J66" s="71"/>
+      <c r="K66" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="86">
+    <row r="67" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="78">
         <v>57</v>
       </c>
-      <c r="B67" s="85"/>
-      <c r="C67" s="78"/>
-      <c r="D67" s="78"/>
-      <c r="E67" s="81"/>
-      <c r="F67" s="82"/>
-      <c r="G67" s="76"/>
-      <c r="H67" s="81"/>
-      <c r="I67" s="60" t="str">
+      <c r="B67" s="77"/>
+      <c r="C67" s="73"/>
+      <c r="D67" s="73"/>
+      <c r="E67" s="126"/>
+      <c r="F67" s="131"/>
+      <c r="G67" s="130"/>
+      <c r="H67" s="74"/>
+      <c r="I67" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J67" s="73"/>
-      <c r="K67" s="60" t="str">
+      <c r="J67" s="71"/>
+      <c r="K67" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="86">
+    <row r="68" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="78">
         <v>58</v>
       </c>
-      <c r="B68" s="85"/>
-      <c r="C68" s="78"/>
-      <c r="D68" s="78"/>
-      <c r="E68" s="81"/>
-      <c r="F68" s="82"/>
-      <c r="G68" s="76"/>
-      <c r="H68" s="81"/>
-      <c r="I68" s="60" t="str">
+      <c r="B68" s="77"/>
+      <c r="C68" s="73"/>
+      <c r="D68" s="73"/>
+      <c r="E68" s="126"/>
+      <c r="F68" s="131"/>
+      <c r="G68" s="130"/>
+      <c r="H68" s="74"/>
+      <c r="I68" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J68" s="73"/>
-      <c r="K68" s="60" t="str">
+      <c r="J68" s="71"/>
+      <c r="K68" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="86">
+    <row r="69" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="78">
         <v>59</v>
       </c>
-      <c r="B69" s="85"/>
-      <c r="C69" s="78"/>
-      <c r="D69" s="78"/>
-      <c r="E69" s="81"/>
-      <c r="F69" s="82"/>
-      <c r="G69" s="76"/>
-      <c r="H69" s="81"/>
-      <c r="I69" s="60" t="str">
+      <c r="B69" s="77"/>
+      <c r="C69" s="73"/>
+      <c r="D69" s="73"/>
+      <c r="E69" s="126"/>
+      <c r="F69" s="131"/>
+      <c r="G69" s="130"/>
+      <c r="H69" s="74"/>
+      <c r="I69" s="136" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="J69" s="73"/>
-      <c r="K69" s="60" t="str">
+      <c r="J69" s="71"/>
+      <c r="K69" s="136" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="87">
+    <row r="70" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="79">
         <v>60</v>
       </c>
-      <c r="B70" s="88"/>
-      <c r="C70" s="89"/>
-      <c r="D70" s="90"/>
-      <c r="E70" s="91"/>
-      <c r="F70" s="92"/>
-      <c r="G70" s="93"/>
-      <c r="H70" s="91"/>
-      <c r="I70" s="62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J70" s="94"/>
-      <c r="K70" s="62" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="103" t="s">
+      <c r="B70" s="80"/>
+      <c r="C70" s="81"/>
+      <c r="D70" s="82"/>
+      <c r="E70" s="127"/>
+      <c r="F70" s="132"/>
+      <c r="G70" s="133"/>
+      <c r="H70" s="83"/>
+      <c r="I70" s="137" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J70" s="84"/>
+      <c r="K70" s="137" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B71" s="103"/>
-      <c r="C71" s="103"/>
+      <c r="B71" s="86"/>
+      <c r="C71" s="86"/>
       <c r="D71" s="56"/>
       <c r="E71" s="37"/>
       <c r="F71" s="37"/>
@@ -3236,7 +3244,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D72" s="36" t="s">
         <v>16</v>
       </c>
@@ -3246,36 +3254,43 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
-      <c r="H73" s="95"/>
-      <c r="I73" s="95"/>
-      <c r="J73" s="95"/>
-      <c r="K73" s="95"/>
-    </row>
-    <row r="74" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H73" s="85"/>
+      <c r="I73" s="85"/>
+      <c r="J73" s="85"/>
+      <c r="K73" s="85"/>
+    </row>
+    <row r="74" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="104"/>
-      <c r="D74" s="104"/>
+      <c r="C74" s="87"/>
+      <c r="D74" s="87"/>
       <c r="E74" s="34"/>
       <c r="F74" s="34"/>
       <c r="G74" s="34"/>
-      <c r="H74" s="105" t="s">
+      <c r="H74" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="I74" s="105"/>
-      <c r="J74" s="105"/>
-      <c r="K74" s="105"/>
+      <c r="I74" s="88"/>
+      <c r="J74" s="88"/>
+      <c r="K74" s="88"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="aySuw4YRe4rzz5kY/TgjpFX/70MiXQTrjzvvmRxVGqM044Cswl1TrK9gDkf+2REIsKgTNhRFCyoKwGuw+Ak/bw==" saltValue="Z5ZjhQ6xosPg4PIqMomKOg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <mergeCells count="21">
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="H74:K74"/>
@@ -3290,13 +3305,6 @@
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.31496062992125984" top="0" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
@@ -3312,50 +3320,50 @@
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="23.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="3.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="23.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="108"/>
+      <c r="K1" s="108"/>
       <c r="L1" s="58"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="125" t="str">
+      <c r="D2" s="118" t="str">
         <f>IF(Hoja1!D2="","",Hoja1!D2)</f>
         <v/>
       </c>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
       <c r="G2" s="58"/>
       <c r="H2" s="58"/>
       <c r="I2" s="22"/>
@@ -3363,23 +3371,23 @@
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="101" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
       <c r="L3" s="59"/>
     </row>
-    <row r="4" spans="1:12" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -3392,79 +3400,79 @@
       <c r="J4" s="24"/>
       <c r="K4" s="23"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="121" t="str">
+      <c r="C5" s="114" t="str">
         <f>IF(Hoja1!C5="","",Hoja1!C5)</f>
         <v/>
       </c>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="121"/>
-      <c r="H5" s="121"/>
-      <c r="I5" s="121"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
       <c r="J5" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="123" t="str">
+      <c r="K5" s="116" t="str">
         <f>IF(Hoja1!K5="","",Hoja1!K5)</f>
         <v>may-ago 2020</v>
       </c>
-      <c r="L5" s="123"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L5" s="116"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="122" t="str">
+      <c r="C6" s="115" t="str">
         <f>IF(Hoja1!C6="","",Hoja1!C6)</f>
         <v/>
       </c>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
       <c r="I6" s="48"/>
       <c r="J6" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="124" t="str">
+      <c r="K6" s="117" t="str">
         <f>IF(Hoja1!K6="","",Hoja1!K6)</f>
         <v/>
       </c>
-      <c r="L6" s="124"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L6" s="117"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="128" t="str">
+      <c r="C7" s="112" t="str">
         <f>IF(Hoja1!C7="","",Hoja1!C7)</f>
         <v/>
       </c>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
       <c r="I7" s="47"/>
       <c r="J7" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="127" t="str">
+      <c r="K7" s="111" t="str">
         <f>IF(Hoja1!K7="","",Hoja1!K7)</f>
         <v/>
       </c>
-      <c r="L7" s="127"/>
-    </row>
-    <row r="8" spans="1:12" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L7" s="111"/>
+    </row>
+    <row r="8" spans="1:12" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -3477,45 +3485,45 @@
       <c r="J8" s="26"/>
       <c r="K8" s="23"/>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="107" t="s">
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="113" t="s">
+      <c r="D9" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="115" t="s">
+      <c r="E9" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="117" t="s">
+      <c r="F9" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="117" t="s">
+      <c r="G9" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="119" t="s">
+      <c r="H9" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="120"/>
-      <c r="J9" s="119" t="s">
+      <c r="I9" s="104"/>
+      <c r="J9" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="120"/>
-    </row>
-    <row r="10" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="108"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="112"/>
-      <c r="D10" s="114"/>
-      <c r="E10" s="116"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="118"/>
+      <c r="K9" s="104"/>
+    </row>
+    <row r="10" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="92"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="49" t="s">
         <v>7</v>
       </c>
@@ -3529,7 +3537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>1</v>
       </c>
@@ -3550,7 +3558,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2</v>
       </c>
@@ -3571,7 +3579,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>3</v>
       </c>
@@ -3592,7 +3600,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>4</v>
       </c>
@@ -3613,7 +3621,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -3634,7 +3642,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>6</v>
       </c>
@@ -3655,7 +3663,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>7</v>
       </c>
@@ -3676,7 +3684,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>8</v>
       </c>
@@ -3697,7 +3705,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>9</v>
       </c>
@@ -3718,7 +3726,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>10</v>
       </c>
@@ -3739,7 +3747,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>11</v>
       </c>
@@ -3760,7 +3768,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>12</v>
       </c>
@@ -3781,7 +3789,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>13</v>
       </c>
@@ -3802,7 +3810,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>14</v>
       </c>
@@ -3823,7 +3831,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>15</v>
       </c>
@@ -3844,7 +3852,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>16</v>
       </c>
@@ -3865,7 +3873,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>17</v>
       </c>
@@ -3886,7 +3894,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>18</v>
       </c>
@@ -3907,7 +3915,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>19</v>
       </c>
@@ -3928,7 +3936,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>20</v>
       </c>
@@ -3949,7 +3957,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>21</v>
       </c>
@@ -3970,7 +3978,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>22</v>
       </c>
@@ -3991,7 +3999,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>23</v>
       </c>
@@ -4012,7 +4020,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>24</v>
       </c>
@@ -4033,7 +4041,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>25</v>
       </c>
@@ -4054,7 +4062,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>26</v>
       </c>
@@ -4075,7 +4083,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>27</v>
       </c>
@@ -4096,7 +4104,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>28</v>
       </c>
@@ -4117,7 +4125,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>29</v>
       </c>
@@ -4138,7 +4146,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>30</v>
       </c>
@@ -4159,7 +4167,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>31</v>
       </c>
@@ -4180,7 +4188,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>32</v>
       </c>
@@ -4201,7 +4209,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>33</v>
       </c>
@@ -4222,7 +4230,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>34</v>
       </c>
@@ -4243,7 +4251,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>35</v>
       </c>
@@ -4264,7 +4272,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>36</v>
       </c>
@@ -4285,7 +4293,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>37</v>
       </c>
@@ -4306,7 +4314,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>38</v>
       </c>
@@ -4327,7 +4335,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>39</v>
       </c>
@@ -4348,7 +4356,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <f>A49+1</f>
         <v>40</v>
@@ -4370,7 +4378,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <f t="shared" ref="A51:A59" si="2">A50+1</f>
         <v>41</v>
@@ -4392,7 +4400,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -4414,7 +4422,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -4436,7 +4444,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -4458,7 +4466,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -4480,7 +4488,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -4502,7 +4510,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -4524,7 +4532,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -4546,7 +4554,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -4568,7 +4576,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="63">
         <v>50</v>
       </c>
@@ -4589,7 +4597,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="63">
         <v>51</v>
       </c>
@@ -4610,7 +4618,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="63">
         <v>52</v>
       </c>
@@ -4631,7 +4639,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="63">
         <v>53</v>
       </c>
@@ -4652,7 +4660,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="63">
         <v>54</v>
       </c>
@@ -4673,7 +4681,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="63">
         <v>55</v>
       </c>
@@ -4694,7 +4702,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="63">
         <v>56</v>
       </c>
@@ -4715,7 +4723,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="63">
         <v>57</v>
       </c>
@@ -4736,7 +4744,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="63">
         <v>58</v>
       </c>
@@ -4757,7 +4765,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="63">
         <v>59</v>
       </c>
@@ -4778,7 +4786,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="38">
         <v>60</v>
       </c>
@@ -4799,12 +4807,12 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="103" t="s">
+    <row r="71" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B71" s="103"/>
-      <c r="C71" s="103"/>
+      <c r="B71" s="86"/>
+      <c r="C71" s="86"/>
       <c r="D71" s="57" t="str">
         <f>IF(Hoja1!D71="","",Hoja1!D71)</f>
         <v/>
@@ -4818,7 +4826,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D72" s="36" t="s">
         <v>16</v>
       </c>
@@ -4828,42 +4836,43 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
-      <c r="H73" s="126"/>
-      <c r="I73" s="126"/>
-      <c r="J73" s="126"/>
-      <c r="K73" s="126"/>
-    </row>
-    <row r="74" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H73" s="113"/>
+      <c r="I73" s="113"/>
+      <c r="J73" s="113"/>
+      <c r="K73" s="113"/>
+    </row>
+    <row r="74" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="104"/>
-      <c r="D74" s="104"/>
+      <c r="C74" s="87"/>
+      <c r="D74" s="87"/>
       <c r="E74" s="34"/>
       <c r="F74" s="34"/>
       <c r="G74" s="34"/>
-      <c r="H74" s="105" t="s">
+      <c r="H74" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="I74" s="105"/>
-      <c r="J74" s="105"/>
-      <c r="K74" s="105"/>
+      <c r="I74" s="88"/>
+      <c r="J74" s="88"/>
+      <c r="K74" s="88"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="4ZD93nVzm9rL2zYD5+NZUY+CFG03nOqkxgoqN87DkG8x0b5pBG8f6t+Jxu9tpr3fP07+rTGqrpKUdQ11mbgabw==" saltValue="CCzYKRkdApDZMuKLtw0r3g==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <mergeCells count="22">
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="H73:K73"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="H74:K74"/>
@@ -4873,13 +4882,12 @@
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="H9:I9"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C7:H7"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.31496062992125984" top="0" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
@@ -4895,88 +4903,88 @@
       <selection activeCell="C6" sqref="C6:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="23.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.88671875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="3.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="23.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="131"/>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="124"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
       <c r="L1" s="53"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="100" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
       <c r="B3" s="22"/>
       <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="132" t="str">
+      <c r="D3" s="125" t="str">
         <f>IF(Hoja1!D2="","",Hoja1!D2)</f>
         <v/>
       </c>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="101" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="109" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -4989,72 +4997,72 @@
       <c r="J5" s="24"/>
       <c r="K5" s="23"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="133" t="str">
+      <c r="C6" s="121" t="str">
         <f>IF(Hoja1!C5="","",Hoja1!C5)</f>
         <v/>
       </c>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="133"/>
-      <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
       <c r="K6" s="21"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="129" t="str">
+      <c r="C7" s="123" t="str">
         <f>IF(Hoja1!C6="","",Hoja1!C6)</f>
         <v/>
       </c>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
       <c r="I7" s="48"/>
       <c r="J7" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="K7" s="130" t="str">
+      <c r="K7" s="122" t="str">
         <f>IF(Hoja1!K5="","",Hoja1!K5)</f>
         <v>may-ago 2020</v>
       </c>
-      <c r="L7" s="130"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L7" s="122"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="133" t="str">
+      <c r="C8" s="121" t="str">
         <f>IF(Hoja1!C7="","",Hoja1!C7)</f>
         <v/>
       </c>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
-      <c r="G8" s="133"/>
-      <c r="H8" s="133"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
       <c r="I8" s="47"/>
       <c r="J8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="130" t="str">
+      <c r="K8" s="122" t="str">
         <f>IF(Hoja1!K7="","",Hoja1!K7)</f>
         <v/>
       </c>
-      <c r="L8" s="130"/>
-    </row>
-    <row r="9" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L8" s="122"/>
+    </row>
+    <row r="9" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -5067,45 +5075,45 @@
       <c r="J9" s="26"/>
       <c r="K9" s="23"/>
     </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="107" t="s">
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="109" t="s">
+      <c r="B10" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="111" t="s">
+      <c r="C10" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="113" t="s">
+      <c r="D10" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="115" t="s">
+      <c r="E10" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="117" t="s">
+      <c r="F10" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="119" t="s">
+      <c r="H10" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="120"/>
-      <c r="J10" s="119" t="s">
+      <c r="I10" s="104"/>
+      <c r="J10" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="120"/>
-    </row>
-    <row r="11" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="108"/>
-      <c r="B11" s="110"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="114"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
+      <c r="K10" s="104"/>
+    </row>
+    <row r="11" spans="1:12" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="92"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="96"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
       <c r="H11" s="49" t="s">
         <v>7</v>
       </c>
@@ -5119,7 +5127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>1</v>
       </c>
@@ -5140,7 +5148,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -5161,7 +5169,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>3</v>
       </c>
@@ -5182,7 +5190,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -5203,7 +5211,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -5224,7 +5232,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>6</v>
       </c>
@@ -5245,7 +5253,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>7</v>
       </c>
@@ -5266,7 +5274,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>8</v>
       </c>
@@ -5287,7 +5295,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>9</v>
       </c>
@@ -5308,7 +5316,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>10</v>
       </c>
@@ -5329,7 +5337,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>11</v>
       </c>
@@ -5350,7 +5358,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>12</v>
       </c>
@@ -5371,7 +5379,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>13</v>
       </c>
@@ -5392,7 +5400,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>14</v>
       </c>
@@ -5413,7 +5421,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>15</v>
       </c>
@@ -5434,7 +5442,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>16</v>
       </c>
@@ -5455,7 +5463,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>17</v>
       </c>
@@ -5476,7 +5484,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>18</v>
       </c>
@@ -5497,7 +5505,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>19</v>
       </c>
@@ -5518,7 +5526,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>20</v>
       </c>
@@ -5539,7 +5547,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>21</v>
       </c>
@@ -5560,7 +5568,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>22</v>
       </c>
@@ -5581,7 +5589,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>23</v>
       </c>
@@ -5602,7 +5610,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>24</v>
       </c>
@@ -5623,7 +5631,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>25</v>
       </c>
@@ -5644,7 +5652,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>26</v>
       </c>
@@ -5665,7 +5673,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>27</v>
       </c>
@@ -5686,7 +5694,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>28</v>
       </c>
@@ -5707,7 +5715,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>29</v>
       </c>
@@ -5728,7 +5736,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>30</v>
       </c>
@@ -5749,7 +5757,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>31</v>
       </c>
@@ -5770,7 +5778,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>32</v>
       </c>
@@ -5791,7 +5799,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>33</v>
       </c>
@@ -5812,7 +5820,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>34</v>
       </c>
@@ -5833,7 +5841,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>35</v>
       </c>
@@ -5854,7 +5862,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>36</v>
       </c>
@@ -5875,7 +5883,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>37</v>
       </c>
@@ -5896,7 +5904,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>38</v>
       </c>
@@ -5917,7 +5925,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>39</v>
       </c>
@@ -5938,7 +5946,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <f>A50+1</f>
         <v>40</v>
@@ -5960,7 +5968,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <f t="shared" ref="A52:A61" si="2">A51+1</f>
         <v>41</v>
@@ -5982,7 +5990,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -6004,7 +6012,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -6026,7 +6034,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -6048,7 +6056,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -6070,7 +6078,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -6092,7 +6100,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -6114,7 +6122,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -6136,7 +6144,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -6158,7 +6166,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="38">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -6180,12 +6188,12 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="134" t="s">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="B62" s="134"/>
-      <c r="C62" s="134"/>
+      <c r="B62" s="119"/>
+      <c r="C62" s="119"/>
       <c r="D62" s="57" t="str">
         <f>IF(Hoja1!D71="","",Hoja1!D71)</f>
         <v/>
@@ -6199,7 +6207,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D63" s="36" t="s">
         <v>16</v>
       </c>
@@ -6209,33 +6217,40 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
-      <c r="H64" s="126"/>
-      <c r="I64" s="126"/>
-      <c r="J64" s="126"/>
-      <c r="K64" s="126"/>
-    </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C65" s="104"/>
-      <c r="D65" s="104"/>
+      <c r="H64" s="113"/>
+      <c r="I64" s="113"/>
+      <c r="J64" s="113"/>
+      <c r="K64" s="113"/>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C65" s="87"/>
+      <c r="D65" s="87"/>
       <c r="E65" s="34"/>
       <c r="F65" s="34"/>
       <c r="G65" s="34"/>
-      <c r="H65" s="135" t="s">
+      <c r="H65" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="I65" s="135"/>
-      <c r="J65" s="135"/>
-      <c r="K65" s="135"/>
+      <c r="I65" s="120"/>
+      <c r="J65" s="120"/>
+      <c r="K65" s="120"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="0pbJ7DWPtSHRxBMlil2Zpc9jYwccwBd33UyxLwdchEToXvvLYwmYGA0JHmhl2WKsOFn7dTwPEoUar2dDV/RWaQ==" saltValue="Gnm8dXeJ6gr0D8NmE+C11A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0"/>
   <mergeCells count="22">
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="C6:I6"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="H64:K64"/>
     <mergeCell ref="C65:D65"/>
@@ -6251,13 +6266,6 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:K10"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="C6:I6"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.31496062992125984" top="0" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>